<commit_message>
antes de modificar la interface-generacion exe ok
</commit_message>
<xml_diff>
--- a/dist/nueva_bobina.xlsx
+++ b/dist/nueva_bobina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,6 +590,289 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2122</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-02-06 23:18</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>ONDA LINER</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2122</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-02-06 23:18</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>ONDA LINER</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2122</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-02-06 23:18</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>ONDA LINER</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2122</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-02-06 23:18</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>ONDA LINER</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2122</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-02-06 23:18</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>ONDA LINER</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
se agregó el reseteo de Sec cuando cambia nro de bobina
</commit_message>
<xml_diff>
--- a/dist/nueva_bobina.xlsx
+++ b/dist/nueva_bobina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -873,6 +873,116 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>231</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2025-02-27 17:43</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>COVERING</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>434</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>85678</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-03-18 14:45</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Antes de Ajustar impresion
</commit_message>
<xml_diff>
--- a/dist/nueva_bobina.xlsx
+++ b/dist/nueva_bobina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -983,6 +983,914 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1771</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>8205</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>86337</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-07-01 14:29</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>296</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>8205</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>86337</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-07-01 14:29</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1763</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>8207</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>86337</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2025-07-01 14:31</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>292</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>8207</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>86337</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2025-07-01 14:31</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1760</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>8209</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>86337</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2025-07-01 14:31</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>295</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>8209</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>86337</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2025-07-01 14:31</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1801</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>8211</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>86337</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2025-07-01 14:31</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>299</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>8211</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>86337</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2025-07-01 14:31</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>555</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3323</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>76767</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2025-07-10 10:16</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>436</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>3323</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>76767</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2025-07-10 10:16</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>578</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>3324</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>76767</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2025-07-10 10:16</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>454</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>3324</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>76767</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2025-07-10 10:16</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>577</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>3325</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>76767</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2025-07-10 10:16</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>434</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>3325</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>76767</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2025-07-10 10:16</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>540</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1278</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>879</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2025-07-28 16:56</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>LINER PER</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1278</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>879</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2025-07-28 16:56</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>LINER PER</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
delay al presionar imprimir ok
</commit_message>
<xml_diff>
--- a/dist/nueva_bobina.xlsx
+++ b/dist/nueva_bobina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2005,6 +2005,63 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>62,5</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>347</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>406</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>14682</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>86845</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2025-08-22 13:11</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>CART.GRIS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>